<commit_message>
menghapus file php excel dan edit document excel jobdesk
</commit_message>
<xml_diff>
--- a/assets/job_desk/job_desk.xlsx
+++ b/assets/job_desk/job_desk.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L JAYA\Danu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\starkit-rinjani\assets\job_desk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F22FC7-ABF2-49A7-A1CD-8808E6E55AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC77E26-FE3C-4D3C-ADBE-FFBE7650CDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3C930731-8E05-49D3-9162-5481FAA265EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -96,70 +93,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Schedule OK"/>
-      <sheetName val="PIC"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="63">
-          <cell r="H63">
-            <v>12</v>
-          </cell>
-          <cell r="I63">
-            <v>36</v>
-          </cell>
-          <cell r="J63">
-            <v>60</v>
-          </cell>
-          <cell r="K63">
-            <v>80</v>
-          </cell>
-          <cell r="L63">
-            <v>92</v>
-          </cell>
-          <cell r="M63">
-            <v>100</v>
-          </cell>
-          <cell r="N63">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="H64">
-            <v>12</v>
-          </cell>
-          <cell r="I64">
-            <v>36</v>
-          </cell>
-          <cell r="J64">
-            <v>60</v>
-          </cell>
-          <cell r="K64">
-            <v>76</v>
-          </cell>
-          <cell r="L64">
-            <v>80</v>
-          </cell>
-          <cell r="M64">
-            <v>80</v>
-          </cell>
-          <cell r="N64">
-            <v>76</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,11 +392,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C357D4-E775-47CC-AD12-085E2828C724}">
-  <dimension ref="A1:CR1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -472,7 +403,7 @@
     <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,246 +451,6 @@
       </c>
       <c r="P1">
         <v>10</v>
-      </c>
-      <c r="Q1">
-        <v>11</v>
-      </c>
-      <c r="R1">
-        <v>12</v>
-      </c>
-      <c r="S1">
-        <v>13</v>
-      </c>
-      <c r="T1">
-        <v>14</v>
-      </c>
-      <c r="U1">
-        <v>15</v>
-      </c>
-      <c r="V1">
-        <v>16</v>
-      </c>
-      <c r="W1">
-        <v>17</v>
-      </c>
-      <c r="X1">
-        <v>18</v>
-      </c>
-      <c r="Y1">
-        <v>19</v>
-      </c>
-      <c r="Z1">
-        <v>20</v>
-      </c>
-      <c r="AA1">
-        <v>21</v>
-      </c>
-      <c r="AB1">
-        <v>22</v>
-      </c>
-      <c r="AC1">
-        <v>23</v>
-      </c>
-      <c r="AD1">
-        <v>24</v>
-      </c>
-      <c r="AE1">
-        <v>25</v>
-      </c>
-      <c r="AF1">
-        <v>26</v>
-      </c>
-      <c r="AG1">
-        <v>27</v>
-      </c>
-      <c r="AH1">
-        <v>28</v>
-      </c>
-      <c r="AI1">
-        <v>29</v>
-      </c>
-      <c r="AJ1">
-        <v>30</v>
-      </c>
-      <c r="AK1">
-        <v>31</v>
-      </c>
-      <c r="AL1">
-        <v>32</v>
-      </c>
-      <c r="AM1">
-        <v>33</v>
-      </c>
-      <c r="AN1">
-        <v>34</v>
-      </c>
-      <c r="AO1">
-        <v>35</v>
-      </c>
-      <c r="AP1">
-        <v>36</v>
-      </c>
-      <c r="AQ1">
-        <v>37</v>
-      </c>
-      <c r="AR1">
-        <v>38</v>
-      </c>
-      <c r="AS1">
-        <v>39</v>
-      </c>
-      <c r="AT1">
-        <v>40</v>
-      </c>
-      <c r="AU1">
-        <v>41</v>
-      </c>
-      <c r="AV1">
-        <v>42</v>
-      </c>
-      <c r="AW1">
-        <v>43</v>
-      </c>
-      <c r="AX1">
-        <v>44</v>
-      </c>
-      <c r="AY1">
-        <v>45</v>
-      </c>
-      <c r="AZ1">
-        <v>46</v>
-      </c>
-      <c r="BA1">
-        <v>47</v>
-      </c>
-      <c r="BB1">
-        <v>48</v>
-      </c>
-      <c r="BC1">
-        <v>49</v>
-      </c>
-      <c r="BD1">
-        <v>50</v>
-      </c>
-      <c r="BE1">
-        <v>51</v>
-      </c>
-      <c r="BF1">
-        <v>52</v>
-      </c>
-      <c r="BG1">
-        <v>53</v>
-      </c>
-      <c r="BH1">
-        <v>54</v>
-      </c>
-      <c r="BI1">
-        <v>55</v>
-      </c>
-      <c r="BJ1">
-        <v>56</v>
-      </c>
-      <c r="BK1">
-        <v>57</v>
-      </c>
-      <c r="BL1">
-        <v>58</v>
-      </c>
-      <c r="BM1">
-        <v>59</v>
-      </c>
-      <c r="BN1">
-        <v>60</v>
-      </c>
-      <c r="BO1">
-        <v>61</v>
-      </c>
-      <c r="BP1">
-        <v>62</v>
-      </c>
-      <c r="BQ1">
-        <v>63</v>
-      </c>
-      <c r="BR1">
-        <v>64</v>
-      </c>
-      <c r="BS1">
-        <v>65</v>
-      </c>
-      <c r="BT1">
-        <v>66</v>
-      </c>
-      <c r="BU1">
-        <v>67</v>
-      </c>
-      <c r="BV1">
-        <v>68</v>
-      </c>
-      <c r="BW1">
-        <v>69</v>
-      </c>
-      <c r="BX1">
-        <v>70</v>
-      </c>
-      <c r="BY1">
-        <v>71</v>
-      </c>
-      <c r="BZ1">
-        <v>72</v>
-      </c>
-      <c r="CA1">
-        <v>73</v>
-      </c>
-      <c r="CB1">
-        <v>74</v>
-      </c>
-      <c r="CC1">
-        <v>75</v>
-      </c>
-      <c r="CD1">
-        <v>76</v>
-      </c>
-      <c r="CE1">
-        <v>77</v>
-      </c>
-      <c r="CF1">
-        <v>78</v>
-      </c>
-      <c r="CG1">
-        <v>79</v>
-      </c>
-      <c r="CH1">
-        <v>80</v>
-      </c>
-      <c r="CI1">
-        <v>81</v>
-      </c>
-      <c r="CJ1">
-        <v>82</v>
-      </c>
-      <c r="CK1">
-        <v>83</v>
-      </c>
-      <c r="CL1">
-        <v>84</v>
-      </c>
-      <c r="CM1">
-        <v>85</v>
-      </c>
-      <c r="CN1">
-        <v>86</v>
-      </c>
-      <c r="CO1">
-        <v>87</v>
-      </c>
-      <c r="CP1">
-        <v>88</v>
-      </c>
-      <c r="CQ1">
-        <v>89</v>
-      </c>
-      <c r="CR1">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fitur import list pekerjaan belumselesai
</commit_message>
<xml_diff>
--- a/assets/job_desk/job_desk.xlsx
+++ b/assets/job_desk/job_desk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\starkit-rinjani\assets\job_desk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC77E26-FE3C-4D3C-ADBE-FFBE7650CDEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29676D3B-E575-4395-94E3-1B5E9F07626C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3C930731-8E05-49D3-9162-5481FAA265EE}"/>
   </bookViews>
@@ -25,15 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Durasi (Hari)</t>
-  </si>
-  <si>
-    <t>Hari ke -&gt;</t>
   </si>
   <si>
     <t>Pekerjaan Utama</t>
@@ -392,65 +386,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C357D4-E775-47CC-AD12-085E2828C724}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:CP1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>2</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
       <c r="J1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="O1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P1">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="Q1">
+        <v>13</v>
+      </c>
+      <c r="R1">
+        <v>14</v>
+      </c>
+      <c r="S1">
+        <v>15</v>
+      </c>
+      <c r="T1">
+        <v>16</v>
+      </c>
+      <c r="U1">
+        <v>17</v>
+      </c>
+      <c r="V1">
+        <v>18</v>
+      </c>
+      <c r="W1">
+        <v>19</v>
+      </c>
+      <c r="X1">
+        <v>20</v>
+      </c>
+      <c r="Y1">
+        <v>21</v>
+      </c>
+      <c r="Z1">
+        <v>22</v>
+      </c>
+      <c r="AA1">
+        <v>23</v>
+      </c>
+      <c r="AB1">
+        <v>24</v>
+      </c>
+      <c r="AC1">
+        <v>25</v>
+      </c>
+      <c r="AD1">
+        <v>26</v>
+      </c>
+      <c r="AE1">
+        <v>27</v>
+      </c>
+      <c r="AF1">
+        <v>28</v>
+      </c>
+      <c r="AG1">
+        <v>29</v>
+      </c>
+      <c r="AH1">
+        <v>30</v>
+      </c>
+      <c r="AI1">
+        <v>31</v>
+      </c>
+      <c r="AJ1">
+        <v>32</v>
+      </c>
+      <c r="AK1">
+        <v>33</v>
+      </c>
+      <c r="AL1">
+        <v>34</v>
+      </c>
+      <c r="AM1">
+        <v>35</v>
+      </c>
+      <c r="AN1">
+        <v>36</v>
+      </c>
+      <c r="AO1">
+        <v>37</v>
+      </c>
+      <c r="AP1">
+        <v>38</v>
+      </c>
+      <c r="AQ1">
+        <v>39</v>
+      </c>
+      <c r="AR1">
+        <v>40</v>
+      </c>
+      <c r="AS1">
+        <v>41</v>
+      </c>
+      <c r="AT1">
+        <v>42</v>
+      </c>
+      <c r="AU1">
+        <v>43</v>
+      </c>
+      <c r="AV1">
+        <v>44</v>
+      </c>
+      <c r="AW1">
+        <v>45</v>
+      </c>
+      <c r="AX1">
+        <v>46</v>
+      </c>
+      <c r="AY1">
+        <v>47</v>
+      </c>
+      <c r="AZ1">
+        <v>48</v>
+      </c>
+      <c r="BA1">
+        <v>49</v>
+      </c>
+      <c r="BB1">
+        <v>50</v>
+      </c>
+      <c r="BC1">
+        <v>51</v>
+      </c>
+      <c r="BD1">
+        <v>52</v>
+      </c>
+      <c r="BE1">
+        <v>53</v>
+      </c>
+      <c r="BF1">
+        <v>54</v>
+      </c>
+      <c r="BG1">
+        <v>55</v>
+      </c>
+      <c r="BH1">
+        <v>56</v>
+      </c>
+      <c r="BI1">
+        <v>57</v>
+      </c>
+      <c r="BJ1">
+        <v>58</v>
+      </c>
+      <c r="BK1">
+        <v>59</v>
+      </c>
+      <c r="BL1">
+        <v>60</v>
+      </c>
+      <c r="BM1">
+        <v>61</v>
+      </c>
+      <c r="BN1">
+        <v>62</v>
+      </c>
+      <c r="BO1">
+        <v>63</v>
+      </c>
+      <c r="BP1">
+        <v>64</v>
+      </c>
+      <c r="BQ1">
+        <v>65</v>
+      </c>
+      <c r="BR1">
+        <v>66</v>
+      </c>
+      <c r="BS1">
+        <v>67</v>
+      </c>
+      <c r="BT1">
+        <v>68</v>
+      </c>
+      <c r="BU1">
+        <v>69</v>
+      </c>
+      <c r="BV1">
+        <v>70</v>
+      </c>
+      <c r="BW1">
+        <v>71</v>
+      </c>
+      <c r="BX1">
+        <v>72</v>
+      </c>
+      <c r="BY1">
+        <v>73</v>
+      </c>
+      <c r="BZ1">
+        <v>74</v>
+      </c>
+      <c r="CA1">
+        <v>75</v>
+      </c>
+      <c r="CB1">
+        <v>76</v>
+      </c>
+      <c r="CC1">
+        <v>77</v>
+      </c>
+      <c r="CD1">
+        <v>78</v>
+      </c>
+      <c r="CE1">
+        <v>79</v>
+      </c>
+      <c r="CF1">
+        <v>80</v>
+      </c>
+      <c r="CG1">
+        <v>81</v>
+      </c>
+      <c r="CH1">
+        <v>82</v>
+      </c>
+      <c r="CI1">
+        <v>83</v>
+      </c>
+      <c r="CJ1">
+        <v>84</v>
+      </c>
+      <c r="CK1">
+        <v>85</v>
+      </c>
+      <c r="CL1">
+        <v>86</v>
+      </c>
+      <c r="CM1">
+        <v>87</v>
+      </c>
+      <c r="CN1">
+        <v>88</v>
+      </c>
+      <c r="CO1">
+        <v>89</v>
+      </c>
+      <c r="CP1">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>